<commit_message>
found that a hemi-ellipsoid is a better geometric shape to approximate surface area of Porites and Pocillopora juveniles. Made appropriate changes to scripts. Developed cleaner data sheets through R.
</commit_message>
<xml_diff>
--- a/Data/Juveniles/Data/R_juve_resp_size.xlsx
+++ b/Data/Juveniles/Data/R_juve_resp_size.xlsx
@@ -1,21 +1,166 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina Bean\Documents\Projects\Metabolic_scaling\Data\Juveniles\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4580138-E04F-40BC-ACC2-DBFC7AAB3F6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="1040" windowWidth="18820" windowHeight="9160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Dry_weight.g</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Max.mm</t>
+  </si>
+  <si>
+    <t>Min.mm</t>
+  </si>
+  <si>
+    <t>Height.mm</t>
+  </si>
+  <si>
+    <t>micromol.coral.min</t>
+  </si>
+  <si>
+    <t>std.error</t>
+  </si>
+  <si>
+    <t>p.value.x</t>
+  </si>
+  <si>
+    <t>adj.r.squared</t>
+  </si>
+  <si>
+    <t>SA.cm2.hemi</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Pocillopora</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Porites</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>#Collected corals on 11/08/2020</t>
+  </si>
+  <si>
+    <t>#Preserved corals in 10% formalin for 48 hours</t>
+  </si>
+  <si>
+    <t>#Decalcified corals in 5% HCL over multiple days</t>
+  </si>
+  <si>
+    <t>#Delayed darkness from night of 11/08 (sunset 18:10)</t>
+  </si>
+  <si>
+    <t>#Corals dark acclimated from 14 hrs 24 min - 53 hrs 37 min</t>
+  </si>
+  <si>
+    <t>#Temp ~27C</t>
+  </si>
+  <si>
+    <t>#Chamber 240 mL</t>
+  </si>
+  <si>
+    <t>#Salinity 34 ppt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#SA.cm2.hemi: Surface area of coral assuming the shape of a hemi-ellipsoid= (2*3.14*height*radius1*radius2)
+and getting more accurate estimates by relating geometric surface area to wax dipped surface area from calibration curve. </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,10 +197,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -63,6 +211,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +265,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +297,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +349,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,94 +542,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Dry_weight.g</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Max</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Min</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Height</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>micromol.coral.min</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>std.error</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>p.value.x</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>adj.r.squared</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>SA.cm2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>0.01369999999999999</v>
+        <v>1.369999999999999E-2</v>
       </c>
       <c r="C2">
         <v>11092020</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D2" t="s">
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="F2">
         <v>9.4</v>
@@ -446,82 +610,74 @@
         <v>17</v>
       </c>
       <c r="H2">
-        <v>0.08669630477913377</v>
+        <v>8.6696304779133773E-2</v>
       </c>
       <c r="I2">
-        <v>0.0003937560167649883</v>
+        <v>3.9375601676498831E-4</v>
       </c>
       <c r="J2">
-        <v>5.42970372581434e-263</v>
+        <v>5.4297037258143403E-263</v>
       </c>
       <c r="K2">
-        <v>0.996441232325251</v>
+        <v>0.99644123232525095</v>
       </c>
       <c r="L2">
-        <v>21.67900588</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+        <v>7.6063617480000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>0.01250000000000001</v>
+        <v>1.2500000000000009E-2</v>
       </c>
       <c r="C3">
         <v>11092020</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D3" t="s">
+        <v>13</v>
       </c>
       <c r="E3">
         <v>21.2</v>
       </c>
       <c r="F3">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="G3">
         <v>14.7</v>
       </c>
       <c r="H3">
-        <v>0.08913537157835927</v>
+        <v>8.9135371578359268E-2</v>
       </c>
       <c r="I3">
-        <v>0.0004284857906466418</v>
+        <v>4.2848579064664179E-4</v>
       </c>
       <c r="J3">
-        <v>1.510482802882762e-254</v>
+        <v>1.510482802882762E-254</v>
       </c>
       <c r="K3">
-        <v>0.9960489697923738</v>
+        <v>0.99604896979237378</v>
       </c>
       <c r="L3">
-        <v>25.8426502446</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+        <v>13.8768118776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>0.04959999999999998</v>
+        <v>4.9599999999999977E-2</v>
       </c>
       <c r="C4">
         <v>11092020</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D4" t="s">
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="F4">
         <v>29.1</v>
@@ -533,34 +689,30 @@
         <v>0.2614990607363803</v>
       </c>
       <c r="I4">
-        <v>0.0009517840650569054</v>
+        <v>9.517840650569054E-4</v>
       </c>
       <c r="J4">
-        <v>1.07500691696613e-165</v>
+        <v>1.0750069169661301E-165</v>
       </c>
       <c r="K4">
-        <v>0.9985731547262117</v>
+        <v>0.99857315472621166</v>
       </c>
       <c r="L4">
-        <v>89.56116532110001</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+        <v>80.78038169940001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>0.0108</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="C5">
         <v>11102020</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D5" t="s">
+        <v>13</v>
       </c>
       <c r="E5">
         <v>16.7</v>
@@ -572,37 +724,33 @@
         <v>14</v>
       </c>
       <c r="H5">
-        <v>0.05636682361184571</v>
+        <v>5.6366823611845709E-2</v>
       </c>
       <c r="I5">
-        <v>0.0002353465351341302</v>
+        <v>2.353465351341302E-4</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.997314113631979</v>
+        <v>0.99731411363197897</v>
       </c>
       <c r="L5">
-        <v>21.487720534</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+        <v>10.17139886</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>0.0343</v>
+        <v>3.4299999999999997E-2</v>
       </c>
       <c r="C6">
         <v>11092020</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
       <c r="E6">
         <v>28.6</v>
@@ -614,37 +762,33 @@
         <v>22.4</v>
       </c>
       <c r="H6">
-        <v>0.1882476877636245</v>
+        <v>0.18824768776362449</v>
       </c>
       <c r="I6">
-        <v>0.0007848963981419543</v>
+        <v>7.8489639814195429E-4</v>
       </c>
       <c r="J6">
-        <v>7.333485135709341e-187</v>
+        <v>7.3334851357093407E-187</v>
       </c>
       <c r="K6">
-        <v>0.9978034095848523</v>
+        <v>0.99780340958485225</v>
       </c>
       <c r="L6">
-        <v>50.499331344</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+        <v>34.264752121599997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>0.009099999999999997</v>
+        <v>9.099999999999997E-3</v>
       </c>
       <c r="C7">
         <v>11102020</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D7" t="s">
+        <v>13</v>
       </c>
       <c r="E7">
         <v>16.5</v>
@@ -656,37 +800,33 @@
         <v>17</v>
       </c>
       <c r="H7">
-        <v>0.04149704827319184</v>
+        <v>4.1497048273191839E-2</v>
       </c>
       <c r="I7">
-        <v>0.0004204703932845826</v>
+        <v>4.2047039328458263E-4</v>
       </c>
       <c r="J7">
-        <v>8.204489189174987e-259</v>
+        <v>8.2044891891749866E-259</v>
       </c>
       <c r="K7">
-        <v>0.9895577829824059</v>
+        <v>0.98955778298240593</v>
       </c>
       <c r="L7">
-        <v>24.466306636</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+        <v>10.839196005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>0.04189999999999999</v>
+        <v>4.1899999999999993E-2</v>
       </c>
       <c r="C8">
         <v>11102020</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D8" t="s">
+        <v>13</v>
       </c>
       <c r="E8">
         <v>32</v>
@@ -698,40 +838,36 @@
         <v>28.3</v>
       </c>
       <c r="H8">
-        <v>0.2659443172417448</v>
+        <v>0.26594431724174478</v>
       </c>
       <c r="I8">
-        <v>0.0009461794900233823</v>
+        <v>9.4617949002338234E-4</v>
       </c>
       <c r="J8">
-        <v>4.242643264710473e-195</v>
+        <v>4.2426432647104733E-195</v>
       </c>
       <c r="K8">
-        <v>0.9985482173760106</v>
+        <v>0.99854821737601063</v>
       </c>
       <c r="L8">
-        <v>82.6184181439</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+        <v>74.392422816000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>20</v>
       </c>
       <c r="B9">
-        <v>0.0058</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="C9">
         <v>11102020</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D9" t="s">
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="F9">
         <v>12.4</v>
@@ -740,37 +876,33 @@
         <v>10.5</v>
       </c>
       <c r="H9">
-        <v>0.02860404705128479</v>
+        <v>2.8604047051284789E-2</v>
       </c>
       <c r="I9">
-        <v>0.0005412082125922535</v>
+        <v>5.4120821259225353E-4</v>
       </c>
       <c r="J9">
-        <v>4.926667459075362e-178</v>
+        <v>4.9266674590753618E-178</v>
       </c>
       <c r="K9">
-        <v>0.9784563233587514</v>
+        <v>0.97845632335875143</v>
       </c>
       <c r="L9">
-        <v>14.1072942675</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+        <v>5.6976314220000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>0.0243</v>
+        <v>2.4299999999999999E-2</v>
       </c>
       <c r="C10">
         <v>11102020</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D10" t="s">
+        <v>13</v>
       </c>
       <c r="E10">
         <v>23.1</v>
@@ -782,37 +914,33 @@
         <v>20.3</v>
       </c>
       <c r="H10">
-        <v>0.09730687051300167</v>
+        <v>9.7306870513001673E-2</v>
       </c>
       <c r="I10">
-        <v>0.0004794772019092978</v>
+        <v>4.7947720190929778E-4</v>
       </c>
       <c r="J10">
-        <v>2.837226988263298e-261</v>
+        <v>2.8372269882632979E-261</v>
       </c>
       <c r="K10">
-        <v>0.9967721889669866</v>
+        <v>0.99677218896698661</v>
       </c>
       <c r="L10">
-        <v>42.89892692960002</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+        <v>27.960903177900001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>0.0121</v>
+        <v>1.21E-2</v>
       </c>
       <c r="C11">
         <v>11092020</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D11" t="s">
+        <v>13</v>
       </c>
       <c r="E11">
         <v>18.3</v>
@@ -824,37 +952,33 @@
         <v>12.8</v>
       </c>
       <c r="H11">
-        <v>0.09737390856219952</v>
+        <v>9.7373908562199518E-2</v>
       </c>
       <c r="I11">
-        <v>0.0003928165957391577</v>
+        <v>3.928165957391577E-4</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0.996164699841617</v>
+        <v>0.99616469984161704</v>
       </c>
       <c r="L11">
-        <v>20.2871772672</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+        <v>9.8908191360000011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>23</v>
       </c>
       <c r="B12">
-        <v>0.0315</v>
+        <v>3.15E-2</v>
       </c>
       <c r="C12">
         <v>11092020</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Pocillopora</t>
-        </is>
+      <c r="D12" t="s">
+        <v>13</v>
       </c>
       <c r="E12">
         <v>26.5</v>
@@ -866,37 +990,33 @@
         <v>18.8</v>
       </c>
       <c r="H12">
-        <v>0.1730949054555671</v>
+        <v>0.17309490545556711</v>
       </c>
       <c r="I12">
-        <v>0.0003745516917434484</v>
+        <v>3.7455169174344842E-4</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0.9991022197084635</v>
+        <v>0.99910221970846347</v>
       </c>
       <c r="L12">
-        <v>41.61276069840001</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+        <v>28.176254002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>24</v>
       </c>
       <c r="B13">
-        <v>0.005500000000000005</v>
+        <v>5.5000000000000049E-3</v>
       </c>
       <c r="C13">
         <v>11092020</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D13" t="s">
+        <v>25</v>
       </c>
       <c r="E13">
         <v>12.5</v>
@@ -905,40 +1025,36 @@
         <v>9.4</v>
       </c>
       <c r="G13">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H13">
-        <v>0.04851006230524317</v>
+        <v>4.8510062305243171E-2</v>
       </c>
       <c r="I13">
-        <v>0.0003109015147825525</v>
+        <v>3.1090151478255251E-4</v>
       </c>
       <c r="J13">
-        <v>1.282222513225828e-288</v>
+        <v>1.282222513225828E-288</v>
       </c>
       <c r="K13">
-        <v>0.992297578616088</v>
+        <v>0.99229757861608803</v>
       </c>
       <c r="L13">
-        <v>4.9013379096</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+        <v>1.8344194000000009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>0.0645</v>
+        <v>6.4500000000000002E-2</v>
       </c>
       <c r="C14">
         <v>11092020</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D14" t="s">
+        <v>25</v>
       </c>
       <c r="E14">
         <v>35</v>
@@ -950,37 +1066,33 @@
         <v>18.5</v>
       </c>
       <c r="H14">
-        <v>0.1164890492575447</v>
+        <v>0.11648904925754471</v>
       </c>
       <c r="I14">
-        <v>0.0008958775681612859</v>
+        <v>8.9587756816128592E-4</v>
       </c>
       <c r="J14">
-        <v>9.477492683225426e-146</v>
+        <v>9.4774926832254257E-146</v>
       </c>
       <c r="K14">
         <v>0.9933396575050657</v>
       </c>
       <c r="L14">
-        <v>26.86554743050001</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+        <v>25.386927475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
       </c>
       <c r="B15">
-        <v>0.0441</v>
+        <v>4.41E-2</v>
       </c>
       <c r="C15">
         <v>11102020</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D15" t="s">
+        <v>25</v>
       </c>
       <c r="E15">
         <v>18.3</v>
@@ -992,37 +1104,33 @@
         <v>18</v>
       </c>
       <c r="H15">
-        <v>0.08080747445071621</v>
+        <v>8.0807474450716205E-2</v>
       </c>
       <c r="I15">
-        <v>0.000412110072693059</v>
+        <v>4.1211007269305902E-4</v>
       </c>
       <c r="J15">
-        <v>3.575334537341145e-276</v>
+        <v>3.5753345373411449E-276</v>
       </c>
       <c r="K15">
-        <v>0.9965966967872915</v>
+        <v>0.99659669678729146</v>
       </c>
       <c r="L15">
-        <v>16.297101144</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+        <v>10.109921741999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>28</v>
       </c>
       <c r="B16">
-        <v>0.0565</v>
+        <v>5.6500000000000002E-2</v>
       </c>
       <c r="C16">
         <v>11102020</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D16" t="s">
+        <v>25</v>
       </c>
       <c r="E16">
         <v>33.6</v>
@@ -1037,34 +1145,30 @@
         <v>0.1007730338316362</v>
       </c>
       <c r="I16">
-        <v>0.0005655396901060412</v>
+        <v>5.6553969010604121E-4</v>
       </c>
       <c r="J16">
-        <v>2.863862276517278e-231</v>
+        <v>2.8638622765172781E-231</v>
       </c>
       <c r="K16">
-        <v>0.9961226610739637</v>
+        <v>0.99612266107396374</v>
       </c>
       <c r="L16">
-        <v>24.9461619384</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+        <v>21.817172160000009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>29</v>
       </c>
       <c r="B17">
-        <v>0.002099999999999991</v>
+        <v>2.0999999999999912E-3</v>
       </c>
       <c r="C17">
         <v>11102020</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D17" t="s">
+        <v>25</v>
       </c>
       <c r="E17">
         <v>10</v>
@@ -1076,37 +1180,33 @@
         <v>6.6</v>
       </c>
       <c r="H17">
-        <v>0.007650167665972964</v>
+        <v>7.6501676659729637E-3</v>
       </c>
       <c r="I17">
-        <v>0.00020037146576185</v>
+        <v>2.0037146576185001E-4</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>0.9861752360144857</v>
+        <v>0.98617523601448565</v>
       </c>
       <c r="L17">
-        <v>2.987801876399999</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+        <v>0.91330668000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>30</v>
       </c>
       <c r="B18">
-        <v>0.0202</v>
+        <v>2.0199999999999999E-2</v>
       </c>
       <c r="C18">
         <v>11102020</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D18" t="s">
+        <v>25</v>
       </c>
       <c r="E18">
         <v>22.4</v>
@@ -1118,37 +1218,33 @@
         <v>9</v>
       </c>
       <c r="H18">
-        <v>0.05583625434764659</v>
+        <v>5.5836254347646587E-2</v>
       </c>
       <c r="I18">
-        <v>0.0002720572658953902</v>
+        <v>2.7205726589539021E-4</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0.9967425329990428</v>
+        <v>0.99674253299904281</v>
       </c>
       <c r="L18">
-        <v>10.208577402</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+        <v>7.9400200319999987</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
       </c>
       <c r="B19">
-        <v>0.04069999999999999</v>
+        <v>4.0699999999999993E-2</v>
       </c>
       <c r="C19">
         <v>11102020</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D19" t="s">
+        <v>25</v>
       </c>
       <c r="E19">
         <v>24.1</v>
@@ -1160,37 +1256,33 @@
         <v>22.7</v>
       </c>
       <c r="H19">
-        <v>0.1001379082943367</v>
+        <v>0.10013790829433671</v>
       </c>
       <c r="I19">
-        <v>0.0009299457878375571</v>
+        <v>9.2994578783755708E-4</v>
       </c>
       <c r="J19">
-        <v>9.040647211009874e-138</v>
+        <v>9.0406472110098743E-138</v>
       </c>
       <c r="K19">
-        <v>0.9929797781839985</v>
+        <v>0.99297977818399852</v>
       </c>
       <c r="L19">
-        <v>23.7276942171</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>16.499467078999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>32</v>
       </c>
       <c r="B20">
-        <v>0.06010000000000002</v>
+        <v>6.0100000000000021E-2</v>
       </c>
       <c r="C20">
         <v>11092020</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D20" t="s">
+        <v>25</v>
       </c>
       <c r="E20">
         <v>40.4</v>
@@ -1205,34 +1297,30 @@
         <v>0.1032801665495215</v>
       </c>
       <c r="I20">
-        <v>0.0005060484410541721</v>
+        <v>5.0604844105417207E-4</v>
       </c>
       <c r="J20">
-        <v>7.884210434416374e-240</v>
+        <v>7.884210434416374E-240</v>
       </c>
       <c r="K20">
         <v>0.9960226814297326</v>
       </c>
       <c r="L20">
-        <v>21.16639419180001</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+        <v>18.2438083256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>33</v>
       </c>
       <c r="B21">
-        <v>0.03589999999999999</v>
+        <v>3.5899999999999987E-2</v>
       </c>
       <c r="C21">
         <v>11092020</v>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D21" t="s">
+        <v>25</v>
       </c>
       <c r="E21">
         <v>20.2</v>
@@ -1244,61 +1332,120 @@
         <v>12.5</v>
       </c>
       <c r="H21">
-        <v>0.0769386079650021</v>
+        <v>7.6938607965002098E-2</v>
       </c>
       <c r="I21">
-        <v>0.0004800707218784386</v>
+        <v>4.8007072187843862E-4</v>
       </c>
       <c r="J21">
-        <v>3.649464285214999e-207</v>
+        <v>3.6494642852149993E-207</v>
       </c>
       <c r="K21">
-        <v>0.9944111593708658</v>
+        <v>0.99441115937086577</v>
       </c>
       <c r="L21">
-        <v>10.872363825</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+        <v>6.2714434999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>34</v>
       </c>
       <c r="B22">
-        <v>0.0353</v>
+        <v>3.5299999999999998E-2</v>
       </c>
       <c r="C22">
         <v>11092020</v>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Porites</t>
-        </is>
+      <c r="D22" t="s">
+        <v>25</v>
       </c>
       <c r="E22">
         <v>20.7</v>
       </c>
       <c r="F22">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="G22">
         <v>16.2</v>
       </c>
       <c r="H22">
-        <v>0.09174484506187726</v>
+        <v>9.1744845061877259E-2</v>
       </c>
       <c r="I22">
-        <v>0.000574447630008285</v>
+        <v>5.7444763000828497E-4</v>
       </c>
       <c r="J22">
-        <v>1.74756955638354e-182</v>
+        <v>1.74756955638354E-182</v>
       </c>
       <c r="K22">
         <v>0.9949579712444474</v>
       </c>
       <c r="L22">
-        <v>15.3678001518</v>
+        <v>9.8757831203999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF84214-D699-40CC-9BD1-93AB160B369C}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="105.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified figures to reflect change in surface area estimate as a hemi-ellipsoid.
</commit_message>
<xml_diff>
--- a/Data/Juveniles/Data/R_juve_resp_size.xlsx
+++ b/Data/Juveniles/Data/R_juve_resp_size.xlsx
@@ -8,15 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina Bean\Documents\Projects\Metabolic_scaling\Data\Juveniles\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4580138-E04F-40BC-ACC2-DBFC7AAB3F6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9779FCAA-EE45-4BEB-B353-DF2A465556AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1040" windowWidth="18820" windowHeight="9160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="310" yWindow="0" windowWidth="18820" windowHeight="9160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -128,13 +138,7 @@
     <t>9</t>
   </si>
   <si>
-    <t>#Collected corals on 11/08/2020</t>
-  </si>
-  <si>
     <t>#Preserved corals in 10% formalin for 48 hours</t>
-  </si>
-  <si>
-    <t>#Decalcified corals in 5% HCL over multiple days</t>
   </si>
   <si>
     <t>#Delayed darkness from night of 11/08 (sunset 18:10)</t>
@@ -154,6 +158,12 @@
   <si>
     <t xml:space="preserve">#SA.cm2.hemi: Surface area of coral assuming the shape of a hemi-ellipsoid= (2*3.14*height*radius1*radius2)
 and getting more accurate estimates by relating geometric surface area to wax dipped surface area from calibration curve. </t>
+  </si>
+  <si>
+    <t>#Collected corals on 11/08/2020 at 8:10 am</t>
+  </si>
+  <si>
+    <t>#Decalcified corals in 5% HCL over multiple days (1-7 days)</t>
   </si>
 </sst>
 </file>
@@ -545,9 +555,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1395,7 +1420,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1405,47 +1430,47 @@
   <sheetData>
     <row r="1" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checked confidence intervals because they looked too narrow. Used function predict to predict the y given an x and the confidence intervals associated with that estimate. That lined up correctly with the confidence intervals shown on the graph.
</commit_message>
<xml_diff>
--- a/Data/Juveniles/Data/R_juve_resp_size.xlsx
+++ b/Data/Juveniles/Data/R_juve_resp_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina Bean\Documents\Projects\Metabolic_scaling\Data\Juveniles\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9779FCAA-EE45-4BEB-B353-DF2A465556AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EFED44-0B61-40B8-80E2-21E3BAD05486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="310" yWindow="0" windowWidth="18820" windowHeight="9160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="380" windowWidth="14740" windowHeight="9160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>#Decalcified corals in 5% HCL over multiple days (1-7 days)</t>
+  </si>
+  <si>
+    <t>#Finished processing corals after 87 hours 37 min from collection time. Round up to 88</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1417,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF84214-D699-40CC-9BD1-93AB160B369C}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1473,6 +1476,11 @@
         <v>40</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>